<commit_message>
Made changes in test methods to reflect changes in Section methods
Made FIXME noted regarding source access for sub-sections
</commit_message>
<xml_diff>
--- a/Text Processing/Section Options.xlsx
+++ b/Text Processing/Section Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\OneDrive - Queen's University\Python\Projects\EclipseRelated\PyUtilities\Text Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE4B56A-60C6-4BBC-8CE0-3EDDEEAAD83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD2E8B-C989-4CAC-9E3C-56DEBCA8250B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74CD4D07-87D4-4CAB-87C7-7D01DEE1601D}"/>
+    <workbookView xWindow="28680" yWindow="705" windowWidth="19440" windowHeight="15000" xr2:uid="{74CD4D07-87D4-4CAB-87C7-7D01DEE1601D}"/>
   </bookViews>
   <sheets>
     <sheet name="Section Options" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="115">
   <si>
     <t>Section Options</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>[sect.read(source) for sect in (subsection1, subsection2, subsection3)]</t>
+  </si>
+  <si>
+    <t>gen</t>
   </si>
 </sst>
 </file>
@@ -602,10 +605,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1145,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB00DF5A-5DFE-423D-A59E-E4F96DA14264}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,20 +1162,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
@@ -1245,11 +1248,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
@@ -1303,12 +1306,12 @@
       <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
@@ -1374,12 +1377,12 @@
       <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1397,7 +1400,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1466,11 +1469,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
@@ -2107,20 +2110,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A19:A30"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="C25:C27"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
     <mergeCell ref="A7:A18"/>
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="A2:C2"/>
@@ -2129,6 +2118,20 @@
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A19:A30"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C27"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>